<commit_message>
__add sheet License for Shiyousho_Project_Sales.xlsx
</commit_message>
<xml_diff>
--- a/Specifications/Shiyousho_Project_Sales.xlsx
+++ b/Specifications/Shiyousho_Project_Sales.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="360" windowWidth="8295" windowHeight="6885" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="360" windowWidth="8295" windowHeight="6885" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Tổng Quan" sheetId="2" r:id="rId1"/>
@@ -16,6 +16,7 @@
     <sheet name="SalesStatistic" sheetId="7" r:id="rId7"/>
     <sheet name="GoodsStatistic" sheetId="8" r:id="rId8"/>
     <sheet name="User" sheetId="9" r:id="rId9"/>
+    <sheet name="License" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -172,7 +173,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="208">
   <si>
     <t>Tên dự án: Project Sales</t>
   </si>
@@ -1425,6 +1426,31 @@
         <family val="2"/>
       </rPr>
       <t>) sẽ hiện màn hình sau</t>
+    </r>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <r>
+      <t>(Nếu có thể được thì ngh</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t>ĩ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> ra cách mà 1 license đã sử dụng rồi thì không thể sử dụng lại được nữa. </t>
     </r>
     <phoneticPr fontId="5"/>
   </si>
@@ -3945,8 +3971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:E28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -4096,12 +4122,59 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B4:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="16384" width="9" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:3">
+      <c r="B4" s="3">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
+      <c r="C5" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3">
+      <c r="C6" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3">
+      <c r="C7" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3">
+      <c r="C8" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AB291"/>
   <sheetViews>
-    <sheetView topLeftCell="A131" workbookViewId="0">
-      <selection activeCell="E293" sqref="E293"/>
+    <sheetView topLeftCell="A272" workbookViewId="0">
+      <selection activeCell="A287" sqref="A287:N291"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -6038,8 +6111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:L27"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -6130,7 +6203,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A4:T28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
@@ -6309,7 +6382,8 @@
   </sheetData>
   <phoneticPr fontId="5"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="0" copies="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -6317,8 +6391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A5:X29"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="M43" sqref="M43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -6580,8 +6654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:AB53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G52" sqref="G52"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="K55" sqref="K55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -7043,8 +7117,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:S38"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="H47" sqref="H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -7335,8 +7409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:S48"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="I54" sqref="I54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -7650,8 +7724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:V61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K52" sqref="K52"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>

</xml_diff>

<commit_message>
__add sheet new_user mo tả màn hình tạo user và add role cho user
</commit_message>
<xml_diff>
--- a/Specifications/Shiyousho_Project_Sales.xlsx
+++ b/Specifications/Shiyousho_Project_Sales.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="360" windowWidth="8295" windowHeight="6885" activeTab="9"/>
+    <workbookView xWindow="480" yWindow="360" windowWidth="8295" windowHeight="6885" firstSheet="2" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Tổng Quan" sheetId="2" r:id="rId1"/>
@@ -15,10 +15,11 @@
     <sheet name="Invoice" sheetId="6" r:id="rId6"/>
     <sheet name="SalesStatistic" sheetId="7" r:id="rId7"/>
     <sheet name="GoodsStatistic" sheetId="8" r:id="rId8"/>
-    <sheet name="User" sheetId="9" r:id="rId9"/>
+    <sheet name="old_User" sheetId="9" r:id="rId9"/>
     <sheet name="License" sheetId="10" r:id="rId10"/>
+    <sheet name="new_user" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -173,7 +174,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="234">
   <si>
     <t>Tên dự án: Project Sales</t>
   </si>
@@ -1454,19 +1455,135 @@
     </r>
     <phoneticPr fontId="5"/>
   </si>
+  <si>
+    <t>Tạo User</t>
+  </si>
+  <si>
+    <t>Khi người dùng chọn chức năng tạo user trên Menu hoặc màn hình Output User</t>
+  </si>
+  <si>
+    <t>Chỉ có user có role Admin mới được tạo user</t>
+  </si>
+  <si>
+    <t>Màn hình khời tạo:</t>
+  </si>
+  <si>
+    <t>Field username</t>
+  </si>
+  <si>
+    <t>Field password</t>
+  </si>
+  <si>
+    <t>listbox bên trái</t>
+  </si>
+  <si>
+    <t>Hiện tất cả role(principal) hiện có</t>
+  </si>
+  <si>
+    <t>listbox bên phải</t>
+  </si>
+  <si>
+    <t>trống</t>
+  </si>
+  <si>
+    <t>Nút &gt;&gt;</t>
+  </si>
+  <si>
+    <t>Chọn tất cả role bên listbox trái sang listbox phải</t>
+  </si>
+  <si>
+    <t>Nút &gt;</t>
+  </si>
+  <si>
+    <t>Chọn role được chọn bên listbox trái sang listbox phải</t>
+  </si>
+  <si>
+    <t>Nút &lt;&lt;</t>
+  </si>
+  <si>
+    <t>Chọn tất cả role bên listbox phải sang listbox trái</t>
+  </si>
+  <si>
+    <t>Nút &lt;</t>
+  </si>
+  <si>
+    <t>Chọn role được chọn bên listbox phải sang listbox trái</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>**</t>
+  </si>
+  <si>
+    <t>Ngoại lệ</t>
+  </si>
+  <si>
+    <r>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>)(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>**</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Khi không có role nào được chọn sẽ hiện lên Message cảnh báo </t>
+  </si>
+  <si>
+    <t>"Vui lòng chọn role bên trái(phải)"</t>
+  </si>
+  <si>
+    <t>Cả 2 listbox đều cho phép chọn multi select</t>
+  </si>
+  <si>
+    <t>Các nút phía bên trên dòng kẻ là các nút chức năng chung, vui lòng tham khảo đến Common_ function_gui.xls</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="0."/>
+    <numFmt numFmtId="164" formatCode="0."/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -1498,7 +1615,7 @@
     </font>
     <font>
       <sz val="6"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -1548,6 +1665,12 @@
       <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1895,11 +2018,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1961,6 +2084,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3684,6 +3808,49 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>543649</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>95758</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3" descr="EditUser1.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="238125" y="647700"/>
+          <a:ext cx="5182324" cy="3639058"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3975,7 +4142,7 @@
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="16384" width="9" style="2"/>
   </cols>
@@ -4126,11 +4293,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B4:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="16384" width="9" style="2"/>
   </cols>
@@ -4166,6 +4333,140 @@
   </sheetData>
   <phoneticPr fontId="5"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:T22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:20">
+      <c r="A2" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
+      <c r="B3" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
+      <c r="K5" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="L6" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20">
+      <c r="L7" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="L9" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="L10" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20">
+      <c r="L12" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20">
+      <c r="L13" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="T13" s="63" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20">
+      <c r="L14" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20">
+      <c r="L15" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="T15" s="63" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="17" spans="12:14">
+      <c r="L17" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="18" spans="12:14">
+      <c r="N18" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="20" spans="12:14">
+      <c r="L20" s="2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="22" spans="12:14">
+      <c r="L22" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4177,12 +4478,12 @@
       <selection activeCell="A287" sqref="A287:N291"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="3" width="9" style="2"/>
-    <col min="4" max="4" width="10.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="2"/>
-    <col min="6" max="6" width="10.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
@@ -6115,7 +6416,7 @@
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="16384" width="9" style="2"/>
   </cols>
@@ -6207,7 +6508,7 @@
       <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="16384" width="9" style="2"/>
   </cols>
@@ -6391,11 +6692,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A5:X29"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="M43" sqref="M43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="16384" width="9" style="2"/>
   </cols>
@@ -6658,7 +6959,7 @@
       <selection activeCell="K55" sqref="K55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="16384" width="9" style="2"/>
   </cols>
@@ -7121,7 +7422,7 @@
       <selection activeCell="H47" sqref="H47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="16384" width="9" style="2"/>
   </cols>
@@ -7413,7 +7714,7 @@
       <selection activeCell="I54" sqref="I54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="16384" width="9" style="2"/>
   </cols>
@@ -7724,13 +8025,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:V61"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="16384" width="9" style="2"/>
+    <col min="1" max="12" width="9" style="2"/>
+    <col min="13" max="13" width="14.7109375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.85546875" style="2" customWidth="1"/>
+    <col min="15" max="15" width="12" style="2" customWidth="1"/>
+    <col min="16" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:18">

</xml_diff>

<commit_message>
_add cases when >>,>,<<,< are invisible on sheet new_user in Shiyousho_Project_Sales.xlsx
</commit_message>
<xml_diff>
--- a/Specifications/Shiyousho_Project_Sales.xlsx
+++ b/Specifications/Shiyousho_Project_Sales.xlsx
@@ -174,7 +174,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="237">
   <si>
     <t>Tên dự án: Project Sales</t>
   </si>
@@ -1569,7 +1569,16 @@
     <t>Cả 2 listbox đều cho phép chọn multi select</t>
   </si>
   <si>
-    <t>Các nút phía bên trên dòng kẻ là các nút chức năng chung, vui lòng tham khảo đến Common_ function_gui.xls</t>
+    <t>Các nút phía bên trên dòng kẻ là các nút chức năng chung, vui lòng tham khảo đến CommonFunctionGui.xls</t>
+  </si>
+  <si>
+    <t>Khi listbox bên trái trống</t>
+  </si>
+  <si>
+    <t>Trạng thái invisible các nút</t>
+  </si>
+  <si>
+    <t>Khi listbox bên phải trống</t>
   </si>
 </sst>
 </file>
@@ -4338,10 +4347,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:T22"/>
+  <dimension ref="A2:T27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="R27" sqref="R27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -4437,7 +4446,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="17" spans="12:14">
+    <row r="17" spans="11:14">
       <c r="L17" s="2" t="s">
         <v>228</v>
       </c>
@@ -4448,19 +4457,56 @@
         <v>230</v>
       </c>
     </row>
-    <row r="18" spans="12:14">
+    <row r="18" spans="11:14">
       <c r="N18" s="2" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="20" spans="12:14">
+    <row r="20" spans="11:14">
       <c r="L20" s="2" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="22" spans="12:14">
+    <row r="22" spans="11:14">
       <c r="L22" s="2" t="s">
         <v>233</v>
+      </c>
+    </row>
+    <row r="23" spans="11:14">
+      <c r="K23" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="24" spans="11:14">
+      <c r="L24" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="N24" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="25" spans="11:14">
+      <c r="L25" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="N25" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="26" spans="11:14">
+      <c r="L26" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="N26" s="2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="27" spans="11:14">
+      <c r="L27" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="N27" s="2" t="s">
+        <v>236</v>
       </c>
     </row>
   </sheetData>

</xml_diff>